<commit_message>
UI-784: Updated the test plan with the new carrier settings
</commit_message>
<xml_diff>
--- a/design/Test Plan/TestPlan.xlsx
+++ b/design/Test Plan/TestPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,15 +522,9 @@
     <t>Click on the "Carrier" tab</t>
   </si>
   <si>
-    <t>The carrier tab opens, containing an info box and a dropdown of carrier settings.</t>
-  </si>
-  <si>
     <t>Select a different Carrier setting then click on Update</t>
   </si>
   <si>
-    <t>The carrier setting is updated, and a green toast appears in the top-right corner of the page to inform the user.</t>
-  </si>
-  <si>
     <t>Disable/Enable an account</t>
   </si>
   <si>
@@ -580,6 +574,12 @@
   </si>
   <si>
     <t>The account is not deleted and an error message is displayed to the user</t>
+  </si>
+  <si>
+    <t>The carrier tab opens, containing 3 boxes (this is the default configuration, if whitelabel is on and they customize the reseller option, it could change this behavior)</t>
+  </si>
+  <si>
+    <t>Before clicking on one of the button the Update button was disabled, when you changed the selected button, it enabled the "Update" button, and then after you saved it, it re-disabled it!</t>
   </si>
 </sst>
 </file>
@@ -2536,35 +2536,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.28515625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="48.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.33203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="48.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" ht="26.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="35"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="42" t="s">
         <v>3</v>
       </c>
@@ -2591,14 +2591,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="37"/>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="36" t="s">
         <v>19</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="36" t="s">
         <v>20</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C10" s="11" t="s">
         <v>4</v>
       </c>
@@ -2631,7 +2631,7 @@
       <c r="J10" s="12"/>
       <c r="L10"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="C11" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>1</v>
@@ -2647,7 +2647,7 @@
       <c r="J11" s="17"/>
       <c r="L11"/>
     </row>
-    <row r="12" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="28" t="s">
         <v>9</v>
       </c>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="L12"/>
     </row>
-    <row r="13" spans="2:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="J13" s="29"/>
     </row>
-    <row r="14" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C14" s="19" t="s">
         <v>10</v>
       </c>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="J14" s="19"/>
     </row>
-    <row r="15" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C15" s="19" t="str">
         <f>CHAR(CODE(C14)+1)</f>
         <v>B</v>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="J15" s="19"/>
     </row>
-    <row r="16" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C16" s="19" t="str">
         <f>CHAR(CODE(C15)+1)</f>
         <v>C</v>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="J16" s="19"/>
     </row>
-    <row r="17" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C17" s="19" t="str">
         <f t="shared" ref="C17:C21" si="0">CHAR(CODE(C16)+1)</f>
         <v>D</v>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="J17" s="19"/>
     </row>
-    <row r="18" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C18" s="19" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
@@ -2782,7 +2782,7 @@
       </c>
       <c r="J18" s="19"/>
     </row>
-    <row r="19" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" s="19" t="str">
         <f t="shared" si="0"/>
         <v>F</v>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="J19" s="19"/>
     </row>
-    <row r="20" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C20" s="19" t="str">
         <f t="shared" si="0"/>
         <v>G</v>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="J20" s="19"/>
     </row>
-    <row r="21" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C21" s="19" t="str">
         <f t="shared" si="0"/>
         <v>H</v>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="J21" s="19"/>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C23" s="11" t="s">
         <v>4</v>
       </c>
@@ -2856,7 +2856,7 @@
       <c r="J23" s="12"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C24" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>2</v>
@@ -2872,7 +2872,7 @@
       <c r="J24" s="17"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="28" t="s">
         <v>9</v>
       </c>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="L25"/>
     </row>
-    <row r="26" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="J26" s="29"/>
     </row>
-    <row r="27" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C27" s="19" t="s">
         <v>10</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="J27" s="19"/>
     </row>
-    <row r="28" spans="3:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C28" s="19" t="str">
         <f>CHAR(CODE(C27)+1)</f>
         <v>B</v>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="J28" s="19"/>
     </row>
-    <row r="29" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C29" s="19" t="str">
         <f>CHAR(CODE(C28)+1)</f>
         <v>C</v>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="J29" s="19"/>
     </row>
-    <row r="30" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C30" s="19" t="str">
         <f>CHAR(CODE(C29)+1)</f>
         <v>D</v>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="J30" s="19"/>
     </row>
-    <row r="31" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C31" s="19" t="str">
         <f>CHAR(CODE(C30)+1)</f>
         <v>E</v>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="J31" s="19"/>
     </row>
-    <row r="32" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C32" s="19" t="str">
         <f t="shared" ref="C32:C35" si="1">CHAR(CODE(C31)+1)</f>
         <v>F</v>
@@ -3026,7 +3026,7 @@
       </c>
       <c r="J32" s="19"/>
     </row>
-    <row r="33" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C33" s="19" t="str">
         <f t="shared" si="1"/>
         <v>G</v>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="J33" s="19"/>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C34" s="19" t="str">
         <f t="shared" si="1"/>
         <v>H</v>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C35" s="19" t="str">
         <f t="shared" si="1"/>
         <v>I</v>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C36" s="19" t="str">
         <f t="shared" ref="C36:C40" si="2">CHAR(CODE(C35)+1)</f>
         <v>J</v>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="J36" s="19"/>
     </row>
-    <row r="37" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C37" s="19" t="str">
         <f t="shared" si="2"/>
         <v>K</v>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="J37" s="19"/>
     </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C38" s="19" t="str">
         <f t="shared" si="2"/>
         <v>L</v>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="J38" s="19"/>
     </row>
-    <row r="39" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C39" s="19" t="str">
         <f t="shared" si="2"/>
         <v>M</v>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="J39" s="19"/>
     </row>
-    <row r="40" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C40" s="19" t="str">
         <f t="shared" si="2"/>
         <v>N</v>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="J40" s="19"/>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C42" s="11" t="s">
         <v>4</v>
       </c>
@@ -3193,7 +3193,7 @@
       <c r="J42" s="12"/>
       <c r="L42"/>
     </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C43" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>3</v>
@@ -3209,7 +3209,7 @@
       <c r="J43" s="17"/>
       <c r="L43"/>
     </row>
-    <row r="44" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="28" t="s">
         <v>9</v>
       </c>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="L44"/>
     </row>
-    <row r="45" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="J45" s="29"/>
     </row>
-    <row r="46" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C46" s="19" t="s">
         <v>10</v>
       </c>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C47" s="19" t="str">
         <f>CHAR(CODE(C46)+1)</f>
         <v>B</v>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C48" s="19" t="str">
         <f t="shared" ref="C48:C57" si="3">CHAR(CODE(C47)+1)</f>
         <v>C</v>
@@ -3310,7 +3310,7 @@
       </c>
       <c r="J48" s="19"/>
     </row>
-    <row r="49" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C49" s="19" t="str">
         <f t="shared" si="3"/>
         <v>D</v>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="J49" s="19"/>
     </row>
-    <row r="50" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C50" s="19" t="str">
         <f t="shared" si="3"/>
         <v>E</v>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="J50" s="19"/>
     </row>
-    <row r="51" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C51" s="19" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="J51" s="19"/>
     </row>
-    <row r="52" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C52" s="19" t="str">
         <f t="shared" si="3"/>
         <v>G</v>
@@ -3394,7 +3394,7 @@
       </c>
       <c r="J52" s="19"/>
     </row>
-    <row r="53" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C53" s="19" t="str">
         <f t="shared" si="3"/>
         <v>H</v>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="J53" s="19"/>
     </row>
-    <row r="54" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C54" s="19" t="str">
         <f t="shared" si="3"/>
         <v>I</v>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="J54" s="19"/>
     </row>
-    <row r="55" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C55" s="19" t="str">
         <f t="shared" si="3"/>
         <v>J</v>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="J55" s="19"/>
     </row>
-    <row r="56" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C56" s="19" t="str">
         <f t="shared" si="3"/>
         <v>K</v>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="J56" s="19"/>
     </row>
-    <row r="57" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C57" s="19" t="str">
         <f t="shared" si="3"/>
         <v>L</v>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="J57" s="19"/>
     </row>
-    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C59" s="11" t="s">
         <v>4</v>
       </c>
@@ -3514,7 +3514,7 @@
       <c r="J59" s="12"/>
       <c r="L59"/>
     </row>
-    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C60" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>4</v>
@@ -3530,7 +3530,7 @@
       <c r="J60" s="17"/>
       <c r="L60"/>
     </row>
-    <row r="61" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="28" t="s">
         <v>9</v>
       </c>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="L61"/>
     </row>
-    <row r="62" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="29"/>
       <c r="D62" s="29"/>
       <c r="E62" s="29"/>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="J62" s="29"/>
     </row>
-    <row r="63" spans="3:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:12" ht="72" x14ac:dyDescent="0.3">
       <c r="C63" s="19" t="str">
         <f>IF(LEN(C62)=1,CHAR(CODE(C62)+1),"A")</f>
         <v>A</v>
@@ -3590,7 +3590,7 @@
       </c>
       <c r="J63" s="19"/>
     </row>
-    <row r="64" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C64" s="19" t="str">
         <f t="shared" ref="C64:C74" si="4">IF(LEN(C63)=1,CHAR(CODE(C63)+1),"A")</f>
         <v>B</v>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="J64" s="19"/>
     </row>
-    <row r="65" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C65" s="19" t="str">
         <f t="shared" si="4"/>
         <v>C</v>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="J65" s="19"/>
     </row>
-    <row r="66" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C66" s="19" t="str">
         <f t="shared" si="4"/>
         <v>D</v>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="J66" s="19"/>
     </row>
-    <row r="67" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C67" s="19" t="str">
         <f t="shared" si="4"/>
         <v>E</v>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="J67" s="19"/>
     </row>
-    <row r="68" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C68" s="19" t="str">
         <f t="shared" si="4"/>
         <v>F</v>
@@ -3695,7 +3695,7 @@
       </c>
       <c r="J68" s="19"/>
     </row>
-    <row r="69" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C69" s="19" t="str">
         <f t="shared" si="4"/>
         <v>G</v>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="J69" s="19"/>
     </row>
-    <row r="70" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C70" s="19" t="str">
         <f t="shared" si="4"/>
         <v>H</v>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J70" s="19"/>
     </row>
-    <row r="71" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C71" s="19" t="str">
         <f t="shared" si="4"/>
         <v>I</v>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="J71" s="19"/>
     </row>
-    <row r="72" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C72" s="19" t="str">
         <f t="shared" si="4"/>
         <v>J</v>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="J72" s="19"/>
     </row>
-    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C73" s="19" t="str">
         <f t="shared" si="4"/>
         <v>K</v>
@@ -3800,7 +3800,7 @@
       </c>
       <c r="J73" s="19"/>
     </row>
-    <row r="74" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C74" s="19" t="str">
         <f t="shared" si="4"/>
         <v>L</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J74" s="19"/>
     </row>
-    <row r="75" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C75" s="19" t="str">
         <f t="shared" ref="C75:C78" si="5">IF(LEN(C74)=1,CHAR(CODE(C74)+1),"A")</f>
         <v>M</v>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="J75" s="19"/>
     </row>
-    <row r="76" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C76" s="19" t="str">
         <f t="shared" si="5"/>
         <v>N</v>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C77" s="19" t="str">
         <f t="shared" si="5"/>
         <v>O</v>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="J77" s="19"/>
     </row>
-    <row r="78" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C78" s="19" t="str">
         <f t="shared" si="5"/>
         <v>P</v>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="J78" s="19"/>
     </row>
-    <row r="80" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C80" s="11" t="s">
         <v>4</v>
       </c>
@@ -3920,7 +3920,7 @@
       <c r="J80" s="12"/>
       <c r="L80"/>
     </row>
-    <row r="81" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C81" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>5</v>
@@ -3936,7 +3936,7 @@
       <c r="J81" s="17"/>
       <c r="L81"/>
     </row>
-    <row r="82" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C82" s="28" t="s">
         <v>9</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="L82"/>
     </row>
-    <row r="83" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C83" s="29"/>
       <c r="D83" s="29"/>
       <c r="E83" s="29"/>
@@ -3975,7 +3975,7 @@
       </c>
       <c r="J83" s="29"/>
     </row>
-    <row r="84" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C84" s="19" t="str">
         <f>IF(LEN(C83)=1,CHAR(CODE(C83)+1),"A")</f>
         <v>A</v>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="J84" s="19"/>
     </row>
-    <row r="85" spans="3:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:12" ht="72" x14ac:dyDescent="0.3">
       <c r="C85" s="19" t="str">
         <f t="shared" ref="C85:C88" si="6">IF(LEN(C84)=1,CHAR(CODE(C84)+1),"A")</f>
         <v>B</v>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="J85" s="19"/>
     </row>
-    <row r="86" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C86" s="19" t="str">
         <f>IF(LEN(C85)=1,CHAR(CODE(C85)+1),"A")</f>
         <v>C</v>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="J86" s="19"/>
     </row>
-    <row r="87" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C87" s="19" t="str">
         <f t="shared" si="6"/>
         <v>D</v>
@@ -4055,7 +4055,7 @@
       </c>
       <c r="J87" s="19"/>
     </row>
-    <row r="88" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C88" s="19" t="str">
         <f t="shared" si="6"/>
         <v>E</v>
@@ -4076,7 +4076,7 @@
       </c>
       <c r="J88" s="19"/>
     </row>
-    <row r="89" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C89" s="19" t="str">
         <f t="shared" ref="C89" si="7">IF(LEN(C88)=1,CHAR(CODE(C88)+1),"A")</f>
         <v>F</v>
@@ -4097,7 +4097,7 @@
       </c>
       <c r="J89" s="19"/>
     </row>
-    <row r="91" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C91" s="11" t="s">
         <v>4</v>
       </c>
@@ -4112,7 +4112,7 @@
       <c r="J91" s="12"/>
       <c r="L91"/>
     </row>
-    <row r="92" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C92" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>6</v>
@@ -4128,7 +4128,7 @@
       <c r="J92" s="17"/>
       <c r="L92"/>
     </row>
-    <row r="93" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C93" s="28" t="s">
         <v>9</v>
       </c>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="L93"/>
     </row>
-    <row r="94" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C94" s="29"/>
       <c r="D94" s="29"/>
       <c r="E94" s="29"/>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="J94" s="29"/>
     </row>
-    <row r="95" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C95" s="19" t="str">
         <f>IF(LEN(C94)=1,CHAR(CODE(C94)+1),"A")</f>
         <v>A</v>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="J95" s="19"/>
     </row>
-    <row r="96" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C96" s="19" t="str">
         <f t="shared" ref="C96:C100" si="8">IF(LEN(C95)=1,CHAR(CODE(C95)+1),"A")</f>
         <v>B</v>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="J96" s="19"/>
     </row>
-    <row r="97" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C97" s="19" t="str">
         <f t="shared" si="8"/>
         <v>C</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="J97" s="19"/>
     </row>
-    <row r="98" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C98" s="19" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="J98" s="19"/>
     </row>
-    <row r="99" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C99" s="19" t="str">
         <f t="shared" si="8"/>
         <v>E</v>
@@ -4272,7 +4272,7 @@
       </c>
       <c r="J99" s="19"/>
     </row>
-    <row r="100" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C100" s="19" t="str">
         <f t="shared" si="8"/>
         <v>F</v>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="J100" s="19"/>
     </row>
-    <row r="102" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C102" s="11" t="s">
         <v>4</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="J102" s="12"/>
       <c r="L102"/>
     </row>
-    <row r="103" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C103" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>7</v>
@@ -4324,7 +4324,7 @@
       <c r="J103" s="17"/>
       <c r="L103"/>
     </row>
-    <row r="104" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C104" s="28" t="s">
         <v>9</v>
       </c>
@@ -4345,7 +4345,7 @@
       </c>
       <c r="L104"/>
     </row>
-    <row r="105" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C105" s="29"/>
       <c r="D105" s="29"/>
       <c r="E105" s="29"/>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="J105" s="29"/>
     </row>
-    <row r="106" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C106" s="19" t="str">
         <f>IF(LEN(C105)=1,CHAR(CODE(C105)+1),"A")</f>
         <v>A</v>
@@ -4384,7 +4384,7 @@
       </c>
       <c r="J106" s="19"/>
     </row>
-    <row r="107" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C107" s="19" t="str">
         <f t="shared" ref="C107:C112" si="9">IF(LEN(C106)=1,CHAR(CODE(C106)+1),"A")</f>
         <v>B</v>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="J107" s="19"/>
     </row>
-    <row r="108" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C108" s="19" t="str">
         <f t="shared" si="9"/>
         <v>C</v>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="J108" s="19"/>
     </row>
-    <row r="109" spans="3:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C109" s="19" t="str">
         <f t="shared" si="9"/>
         <v>D</v>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="J109" s="19"/>
     </row>
-    <row r="110" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C110" s="19" t="str">
         <f t="shared" si="9"/>
         <v>E</v>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="J110" s="19"/>
     </row>
-    <row r="111" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C111" s="19" t="str">
         <f t="shared" si="9"/>
         <v>F</v>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="J111" s="19"/>
     </row>
-    <row r="112" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C112" s="19" t="str">
         <f t="shared" si="9"/>
         <v>G</v>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="J112" s="19"/>
     </row>
-    <row r="113" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C113" s="24"/>
       <c r="D113" s="25"/>
       <c r="E113" s="25"/>
@@ -4520,7 +4520,7 @@
       <c r="I113" s="27"/>
       <c r="J113" s="24"/>
     </row>
-    <row r="114" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C114" s="11" t="s">
         <v>4</v>
       </c>
@@ -4535,7 +4535,7 @@
       <c r="J114" s="12"/>
       <c r="L114"/>
     </row>
-    <row r="115" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C115" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>8</v>
@@ -4551,7 +4551,7 @@
       <c r="J115" s="17"/>
       <c r="L115"/>
     </row>
-    <row r="116" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C116" s="28" t="s">
         <v>9</v>
       </c>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="L116"/>
     </row>
-    <row r="117" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C117" s="29"/>
       <c r="D117" s="29"/>
       <c r="E117" s="29"/>
@@ -4590,7 +4590,7 @@
       </c>
       <c r="J117" s="29"/>
     </row>
-    <row r="118" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C118" s="19" t="str">
         <f>IF(LEN(C117)=1,CHAR(CODE(C117)+1),"A")</f>
         <v>A</v>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="J118" s="19"/>
     </row>
-    <row r="119" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C119" s="19" t="str">
         <f t="shared" ref="C119:C120" si="10">IF(LEN(C118)=1,CHAR(CODE(C118)+1),"A")</f>
         <v>B</v>
@@ -4620,7 +4620,7 @@
         <v>166</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="F119" s="22"/>
       <c r="G119" s="22"/>
@@ -4632,16 +4632,16 @@
       </c>
       <c r="J119" s="19"/>
     </row>
-    <row r="120" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C120" s="19" t="str">
         <f t="shared" si="10"/>
         <v>C</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="F120" s="22"/>
       <c r="G120" s="22"/>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="J120" s="19"/>
     </row>
-    <row r="122" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C122" s="11" t="s">
         <v>4</v>
       </c>
@@ -4668,7 +4668,7 @@
       <c r="J122" s="12"/>
       <c r="L122"/>
     </row>
-    <row r="123" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C123" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>9</v>
@@ -4684,7 +4684,7 @@
       <c r="J123" s="17"/>
       <c r="L123"/>
     </row>
-    <row r="124" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C124" s="28" t="s">
         <v>9</v>
       </c>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="L124"/>
     </row>
-    <row r="125" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C125" s="29"/>
       <c r="D125" s="29"/>
       <c r="E125" s="29"/>
@@ -4723,7 +4723,7 @@
       </c>
       <c r="J125" s="29"/>
     </row>
-    <row r="126" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C126" s="19" t="str">
         <f>IF(LEN(C125)=1,CHAR(CODE(C125)+1),"A")</f>
         <v>A</v>
@@ -4744,7 +4744,7 @@
       </c>
       <c r="J126" s="19"/>
     </row>
-    <row r="127" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C127" s="19" t="str">
         <f t="shared" ref="C127:C128" si="11">IF(LEN(C126)=1,CHAR(CODE(C126)+1),"A")</f>
         <v>B</v>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="J127" s="19"/>
     </row>
-    <row r="128" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C128" s="19" t="str">
         <f t="shared" si="11"/>
         <v>C</v>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="J128" s="19"/>
     </row>
-    <row r="130" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C130" s="11" t="s">
         <v>4</v>
       </c>
@@ -4801,13 +4801,13 @@
       <c r="J130" s="12"/>
       <c r="L130"/>
     </row>
-    <row r="131" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C131" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>10</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E131" s="16"/>
       <c r="F131" s="16"/>
@@ -4817,7 +4817,7 @@
       <c r="J131" s="17"/>
       <c r="L131"/>
     </row>
-    <row r="132" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C132" s="28" t="s">
         <v>9</v>
       </c>
@@ -4838,7 +4838,7 @@
       </c>
       <c r="L132"/>
     </row>
-    <row r="133" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C133" s="29"/>
       <c r="D133" s="29"/>
       <c r="E133" s="29"/>
@@ -4856,7 +4856,7 @@
       </c>
       <c r="J133" s="29"/>
     </row>
-    <row r="134" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C134" s="19" t="str">
         <f>IF(LEN(C133)=1,CHAR(CODE(C133)+1),"A")</f>
         <v>A</v>
@@ -4875,16 +4875,16 @@
       </c>
       <c r="J134" s="19"/>
     </row>
-    <row r="135" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C135" s="19" t="str">
         <f t="shared" ref="C135:C138" si="12">IF(LEN(C134)=1,CHAR(CODE(C134)+1),"A")</f>
         <v>B</v>
       </c>
       <c r="D135" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F135" s="22"/>
       <c r="G135" s="22"/>
@@ -4894,16 +4894,16 @@
       </c>
       <c r="J135" s="19"/>
     </row>
-    <row r="136" spans="3:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C136" s="19" t="str">
         <f t="shared" si="12"/>
         <v>C</v>
       </c>
       <c r="D136" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F136" s="22"/>
       <c r="G136" s="22"/>
@@ -4913,16 +4913,16 @@
       </c>
       <c r="J136" s="19"/>
     </row>
-    <row r="137" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C137" s="19" t="str">
         <f t="shared" si="12"/>
         <v>D</v>
       </c>
       <c r="D137" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F137" s="22"/>
       <c r="G137" s="22"/>
@@ -4932,16 +4932,16 @@
       </c>
       <c r="J137" s="19"/>
     </row>
-    <row r="138" spans="3:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C138" s="19" t="str">
         <f t="shared" si="12"/>
         <v>E</v>
       </c>
       <c r="D138" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E138" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F138" s="22"/>
       <c r="G138" s="22"/>
@@ -4951,7 +4951,7 @@
       </c>
       <c r="J138" s="19"/>
     </row>
-    <row r="140" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C140" s="11" t="s">
         <v>4</v>
       </c>
@@ -4966,13 +4966,13 @@
       <c r="J140" s="12"/>
       <c r="L140"/>
     </row>
-    <row r="141" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C141" s="14">
         <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>11</v>
       </c>
       <c r="D141" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E141" s="16"/>
       <c r="F141" s="16"/>
@@ -4982,7 +4982,7 @@
       <c r="J141" s="17"/>
       <c r="L141"/>
     </row>
-    <row r="142" spans="3:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C142" s="28" t="s">
         <v>9</v>
       </c>
@@ -5003,7 +5003,7 @@
       </c>
       <c r="L142"/>
     </row>
-    <row r="143" spans="3:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:12" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C143" s="29"/>
       <c r="D143" s="29"/>
       <c r="E143" s="29"/>
@@ -5021,13 +5021,13 @@
       </c>
       <c r="J143" s="29"/>
     </row>
-    <row r="144" spans="3:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C144" s="19" t="str">
         <f>IF(LEN(C143)=1,CHAR(CODE(C143)+1),"A")</f>
         <v>A</v>
       </c>
       <c r="D144" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E144" s="21" t="s">
         <v>71</v>
@@ -5040,16 +5040,16 @@
       </c>
       <c r="J144" s="19"/>
     </row>
-    <row r="145" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C145" s="19" t="str">
         <f t="shared" ref="C145:C148" si="13">IF(LEN(C144)=1,CHAR(CODE(C144)+1),"A")</f>
         <v>B</v>
       </c>
       <c r="D145" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E145" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F145" s="22"/>
       <c r="G145" s="22"/>
@@ -5059,16 +5059,16 @@
       </c>
       <c r="J145" s="19"/>
     </row>
-    <row r="146" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C146" s="19" t="str">
         <f t="shared" si="13"/>
         <v>C</v>
       </c>
       <c r="D146" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E146" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F146" s="22"/>
       <c r="G146" s="22"/>
@@ -5078,16 +5078,16 @@
       </c>
       <c r="J146" s="19"/>
     </row>
-    <row r="147" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C147" s="19" t="str">
         <f t="shared" si="13"/>
         <v>D</v>
       </c>
       <c r="D147" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E147" s="21" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F147" s="22"/>
       <c r="G147" s="22"/>
@@ -5097,16 +5097,16 @@
       </c>
       <c r="J147" s="19"/>
     </row>
-    <row r="148" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C148" s="19" t="str">
         <f t="shared" si="13"/>
         <v>E</v>
       </c>
       <c r="D148" s="21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E148" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F148" s="22"/>
       <c r="G148" s="22"/>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="J148" s="19"/>
     </row>
-    <row r="149" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C149" s="19" t="str">
         <f t="shared" ref="C149" si="14">IF(LEN(C148)=1,CHAR(CODE(C148)+1),"A")</f>
         <v>F</v>
@@ -5133,21 +5133,41 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="J61:J62"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="F142:I142"/>
+    <mergeCell ref="J142:J143"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="F116:I116"/>
+    <mergeCell ref="J116:J117"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="E132:E133"/>
+    <mergeCell ref="F132:I132"/>
+    <mergeCell ref="J132:J133"/>
+    <mergeCell ref="C124:C125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F124:I124"/>
+    <mergeCell ref="J124:J125"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="F104:I104"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="D93:D94"/>
+    <mergeCell ref="E93:E94"/>
+    <mergeCell ref="F93:I93"/>
+    <mergeCell ref="J93:J94"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="D82:D83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="F82:I82"/>
+    <mergeCell ref="J82:J83"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="B6:C6"/>
@@ -5160,41 +5180,21 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="D82:D83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="F82:I82"/>
-    <mergeCell ref="J82:J83"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="D93:D94"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="F93:I93"/>
-    <mergeCell ref="J93:J94"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="F104:I104"/>
-    <mergeCell ref="J104:J105"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="D124:D125"/>
-    <mergeCell ref="E124:E125"/>
-    <mergeCell ref="F124:I124"/>
-    <mergeCell ref="J124:J125"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="D132:D133"/>
-    <mergeCell ref="E132:E133"/>
-    <mergeCell ref="F132:I132"/>
-    <mergeCell ref="J132:J133"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="F116:I116"/>
-    <mergeCell ref="J116:J117"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="F142:I142"/>
-    <mergeCell ref="J142:J143"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="J61:J62"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:I21">
     <cfRule type="containsText" dxfId="171" priority="209" operator="containsText" text="P">
@@ -6963,9 +6963,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>CHAR(CODE(A1)+2)</f>
         <v>C</v>
@@ -6989,7 +6989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A13" si="0">CHAR(CODE(A2)+2)</f>
         <v>E</v>
@@ -6999,7 +6999,7 @@
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>G</v>
@@ -7009,7 +7009,7 @@
         <v>H</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>I</v>
@@ -7019,7 +7019,7 @@
         <v>J</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>K</v>
@@ -7029,7 +7029,7 @@
         <v>L</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>M</v>
@@ -7039,7 +7039,7 @@
         <v>N</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>O</v>
@@ -7049,7 +7049,7 @@
         <v>P</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>Q</v>
@@ -7059,7 +7059,7 @@
         <v>R</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>S</v>
@@ -7069,7 +7069,7 @@
         <v>T</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>U</v>
@@ -7079,7 +7079,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>W</v>
@@ -7089,7 +7089,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>Y</v>

</xml_diff>